<commit_message>
Commit modif InputAnnualData et InputDateRetraite
</commit_message>
<xml_diff>
--- a/Input_client/Input Consignes et Infos.xlsx
+++ b/Input_client/Input Consignes et Infos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\audre\Desktop\Retraite\Projet_Outil_Calcul_Retraite\Input_client\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA7426F-E62E-4D34-B467-B8E575614CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F000BFE-F491-4E20-A643-01AA474E43D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9A11F353-A235-40F0-A7E7-264DCBD7306B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>RCI</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>InputAnnualData</t>
-  </si>
-  <si>
-    <t>trimestres : il s'agit des trimestres tous régimes (pour calcul du taux de retraite et détermination carrière longue)</t>
   </si>
   <si>
     <t>InputCumulDroitsParRegime</t>
@@ -114,6 +111,15 @@
   </si>
   <si>
     <t>ATTENTION : il faut bien compléter le tableau jusqu'à l'année de la date de départ en retraite la plus lointaine -&gt; sinon erreur type "donnee Trim AnnualData incorrecte:"</t>
+  </si>
+  <si>
+    <t>trimestres :  trimestres tous régimes (pour calcul du taux de retraite et détermination carrière longue)</t>
+  </si>
+  <si>
+    <t>trimestres RG (trim validés pas encore utilisé dans le calcul + trim cotisés pris en compte pour calcul SAM)</t>
+  </si>
+  <si>
+    <t>ATTENTION : si rachat il faut renseigner les années concernées par le rachat (car ces années ne seront pas pris en compte dans le calcul du SAM)</t>
   </si>
 </sst>
 </file>
@@ -556,7 +562,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -578,10 +584,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -655,10 +661,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8838B833-D836-44D5-A014-38BBE99B9C4C}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,7 +672,7 @@
     <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -674,43 +680,54 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
-        <v>19</v>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -742,10 +759,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit version stable avec nouveau InputAnnualData
</commit_message>
<xml_diff>
--- a/Input_client/Input Consignes et Infos.xlsx
+++ b/Input_client/Input Consignes et Infos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\audre\Desktop\Retraite\Projet_Outil_Calcul_Retraite\Input_client\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F000BFE-F491-4E20-A643-01AA474E43D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA7426F-E62E-4D34-B467-B8E575614CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9A11F353-A235-40F0-A7E7-264DCBD7306B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>RCI</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>InputAnnualData</t>
+  </si>
+  <si>
+    <t>trimestres : il s'agit des trimestres tous régimes (pour calcul du taux de retraite et détermination carrière longue)</t>
   </si>
   <si>
     <t>InputCumulDroitsParRegime</t>
@@ -111,15 +114,6 @@
   </si>
   <si>
     <t>ATTENTION : il faut bien compléter le tableau jusqu'à l'année de la date de départ en retraite la plus lointaine -&gt; sinon erreur type "donnee Trim AnnualData incorrecte:"</t>
-  </si>
-  <si>
-    <t>trimestres :  trimestres tous régimes (pour calcul du taux de retraite et détermination carrière longue)</t>
-  </si>
-  <si>
-    <t>trimestres RG (trim validés pas encore utilisé dans le calcul + trim cotisés pris en compte pour calcul SAM)</t>
-  </si>
-  <si>
-    <t>ATTENTION : si rachat il faut renseigner les années concernées par le rachat (car ces années ne seront pas pris en compte dans le calcul du SAM)</t>
   </si>
 </sst>
 </file>
@@ -562,7 +556,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -584,10 +578,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -661,10 +655,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8838B833-D836-44D5-A014-38BBE99B9C4C}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,7 +666,7 @@
     <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -680,54 +674,43 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -759,10 +742,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>